<commit_message>
modified writers to handle unicode chars and removed commented out obsolete code from various modules
</commit_message>
<xml_diff>
--- a/fixtures/output/01043110000366247_cancer_risk_exposure.xlsx
+++ b/fixtures/output/01043110000366247_cancer_risk_exposure.xlsx
@@ -349,12 +349,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>level</t>
+          <t>Level</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>population</t>
+          <t>Population</t>
         </is>
       </c>
     </row>

</xml_diff>